<commit_message>
AGREGO SEDLAC AL MAIN pre correr todo
</commit_message>
<xml_diff>
--- a/data_management/management/2. harmonization/ENCOVI harmonization/Encovi_comparability across years 2014-2019_MA abril 13.xlsx
+++ b/data_management/management/2. harmonization/ENCOVI harmonization/Encovi_comparability across years 2014-2019_MA abril 13.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wb550905\OneDrive - WBG\Venezuela\ENCOVI\2019\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://worldbankgroup-my.sharepoint.com/personal/macuna_worldbank_org/Documents/Venezuela/ENCOVI/2019/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="56" documentId="13_ncr:1_{77D8A0D9-5B19-40EE-B1A7-A4599F626D1E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{229C022A-4996-4305-963B-CBAA2016F29E}"/>
+  <xr:revisionPtr revIDLastSave="76" documentId="13_ncr:1_{77D8A0D9-5B19-40EE-B1A7-A4599F626D1E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{EE51320D-5CF1-42F6-9BDF-CD0F9DA43934}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="805" firstSheet="3" activeTab="8" xr2:uid="{C17073D6-622F-4055-BD8D-7FC11D1960F9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="805" firstSheet="1" activeTab="6" xr2:uid="{C17073D6-622F-4055-BD8D-7FC11D1960F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Control_entrevista" sheetId="4" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2068" uniqueCount="1288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2069" uniqueCount="1289">
   <si>
     <t>Questions</t>
   </si>
@@ -4369,10 +4369,6 @@
   </si>
   <si>
     <t>s9q29c_8</t>
-  </si>
-  <si>
-    <t>inla_otro 
-(i.e. Ingreso monetario extraordinario)</t>
   </si>
   <si>
     <t>s9q29c_1</t>
@@ -5099,9 +5095,6 @@
     <t>inla_asig_men</t>
   </si>
   <si>
-    <t>inla_otro</t>
-  </si>
-  <si>
     <t>inla_*_cant</t>
   </si>
   <si>
@@ -5252,6 +5245,16 @@
   </si>
   <si>
     <t>¿Quién pagó por el seguro médico? (solo se pregunta si s8q19 = 1 y s8q18=5)</t>
+  </si>
+  <si>
+    <t>inla_extraord
+(i.e. Ingreso monetario extraordinario)</t>
+  </si>
+  <si>
+    <t>inla_otro (i.e. La imputación de ingreso no laboral diferente a ijubi_m)</t>
+  </si>
+  <si>
+    <t>inla_otros</t>
   </si>
 </sst>
 </file>
@@ -5606,7 +5609,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="205">
+  <cellXfs count="211">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -6174,9 +6177,6 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -6203,6 +6203,27 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -6792,10 +6813,10 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="71" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="B15" s="71" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="C15" s="71" t="s">
         <v>168</v>
@@ -7017,10 +7038,10 @@
     </row>
     <row r="30" spans="1:9">
       <c r="A30" s="71" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="B30" s="71" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="C30" s="71"/>
       <c r="D30" s="71"/>
@@ -7115,10 +7136,10 @@
         <v>442</v>
       </c>
       <c r="B37" s="171" t="s">
-        <v>1251</v>
+        <v>1249</v>
       </c>
       <c r="D37" s="10" t="s">
-        <v>1252</v>
+        <v>1250</v>
       </c>
     </row>
   </sheetData>
@@ -7231,7 +7252,7 @@
         <v>402</v>
       </c>
       <c r="B5" s="64" t="s">
-        <v>1286</v>
+        <v>1284</v>
       </c>
       <c r="C5" s="69" t="s">
         <v>407</v>
@@ -7434,13 +7455,13 @@
       <c r="D2" s="61" t="s">
         <v>383</v>
       </c>
-      <c r="E2" s="200" t="s">
+      <c r="E2" s="199" t="s">
         <v>839</v>
       </c>
-      <c r="F2" s="200"/>
-      <c r="G2" s="200"/>
-      <c r="H2" s="200"/>
-      <c r="I2" s="200"/>
+      <c r="F2" s="199"/>
+      <c r="G2" s="199"/>
+      <c r="H2" s="199"/>
+      <c r="I2" s="199"/>
       <c r="J2" s="51"/>
     </row>
     <row r="3" spans="1:10" s="52" customFormat="1" ht="28.8">
@@ -8232,7 +8253,7 @@
       </c>
       <c r="D3" s="69"/>
       <c r="E3" s="71" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="F3" s="71"/>
       <c r="G3" s="142"/>
@@ -8292,7 +8313,7 @@
         <v>728</v>
       </c>
       <c r="F6" s="71" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="G6" s="142"/>
       <c r="H6" s="142"/>
@@ -8786,7 +8807,7 @@
         <v>433</v>
       </c>
       <c r="D4" s="72" t="s">
-        <v>1280</v>
+        <v>1278</v>
       </c>
       <c r="E4" s="71"/>
       <c r="F4" s="71"/>
@@ -8800,7 +8821,7 @@
         <v>434</v>
       </c>
       <c r="D5" s="72" t="s">
-        <v>1280</v>
+        <v>1278</v>
       </c>
       <c r="E5" s="71"/>
       <c r="F5" s="71"/>
@@ -8827,12 +8848,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="37" customFormat="1">
-      <c r="A1" s="201">
+      <c r="A1" s="200">
         <v>2019</v>
       </c>
-      <c r="B1" s="201"/>
-      <c r="C1" s="201"/>
-      <c r="D1" s="202"/>
+      <c r="B1" s="200"/>
+      <c r="C1" s="200"/>
+      <c r="D1" s="201"/>
     </row>
     <row r="2" spans="1:5" s="50" customFormat="1" ht="43.2">
       <c r="A2" s="94" t="s">
@@ -8851,30 +8872,30 @@
     </row>
     <row r="3" spans="1:5" ht="57.6">
       <c r="A3" s="71" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="B3" s="71" t="s">
-        <v>1281</v>
+        <v>1279</v>
       </c>
       <c r="C3" s="72" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="D3" s="71" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="57.6">
       <c r="A4" s="71" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="B4" s="71" t="s">
-        <v>1282</v>
+        <v>1280</v>
       </c>
       <c r="C4" s="72" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="D4" s="72" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
     </row>
   </sheetData>
@@ -8908,13 +8929,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="37" customFormat="1">
-      <c r="A1" s="201">
+      <c r="A1" s="200">
         <v>2019</v>
       </c>
-      <c r="B1" s="201"/>
-      <c r="C1" s="201"/>
-      <c r="D1" s="201"/>
-      <c r="E1" s="202"/>
+      <c r="B1" s="200"/>
+      <c r="C1" s="200"/>
+      <c r="D1" s="200"/>
+      <c r="E1" s="201"/>
       <c r="F1" s="60">
         <v>2018</v>
       </c>
@@ -8932,10 +8953,10 @@
       </c>
     </row>
     <row r="2" spans="1:11" s="50" customFormat="1" ht="43.2">
-      <c r="A2" s="204" t="s">
+      <c r="A2" s="203" t="s">
         <v>129</v>
       </c>
-      <c r="B2" s="204"/>
+      <c r="B2" s="203"/>
       <c r="C2" s="61" t="s">
         <v>128</v>
       </c>
@@ -8953,10 +8974,10 @@
       <c r="K2" s="51"/>
     </row>
     <row r="3" spans="1:11" ht="72">
-      <c r="A3" s="203" t="s">
+      <c r="A3" s="202" t="s">
         <v>885</v>
       </c>
-      <c r="B3" s="203"/>
+      <c r="B3" s="202"/>
       <c r="C3" s="71" t="s">
         <v>899</v>
       </c>
@@ -8983,7 +9004,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="28.8">
-      <c r="A4" s="203" t="s">
+      <c r="A4" s="202" t="s">
         <v>915</v>
       </c>
       <c r="B4" s="70" t="s">
@@ -9015,7 +9036,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="115.2">
-      <c r="A5" s="203"/>
+      <c r="A5" s="202"/>
       <c r="B5" s="70" t="s">
         <v>887</v>
       </c>
@@ -9045,7 +9066,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" ht="144">
-      <c r="A6" s="203"/>
+      <c r="A6" s="202"/>
       <c r="B6" s="70" t="s">
         <v>888</v>
       </c>
@@ -9075,7 +9096,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="144">
-      <c r="A7" s="203"/>
+      <c r="A7" s="202"/>
       <c r="B7" s="70" t="s">
         <v>889</v>
       </c>
@@ -9105,7 +9126,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="187.2">
-      <c r="A8" s="203"/>
+      <c r="A8" s="202"/>
       <c r="B8" s="70" t="s">
         <v>890</v>
       </c>
@@ -9135,7 +9156,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="302.39999999999998">
-      <c r="A9" s="203"/>
+      <c r="A9" s="202"/>
       <c r="B9" s="70" t="s">
         <v>891</v>
       </c>
@@ -9165,7 +9186,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" s="82" customFormat="1" ht="259.2">
-      <c r="A10" s="203"/>
+      <c r="A10" s="202"/>
       <c r="B10" s="86" t="s">
         <v>892</v>
       </c>
@@ -9195,7 +9216,7 @@
       </c>
     </row>
     <row r="11" spans="1:11" ht="187.2">
-      <c r="A11" s="203"/>
+      <c r="A11" s="202"/>
       <c r="B11" s="70" t="s">
         <v>893</v>
       </c>
@@ -9225,7 +9246,7 @@
       </c>
     </row>
     <row r="12" spans="1:11" ht="144">
-      <c r="A12" s="203"/>
+      <c r="A12" s="202"/>
       <c r="B12" s="70" t="s">
         <v>894</v>
       </c>
@@ -9255,7 +9276,7 @@
       </c>
     </row>
     <row r="13" spans="1:11" ht="144">
-      <c r="A13" s="203"/>
+      <c r="A13" s="202"/>
       <c r="B13" s="70" t="s">
         <v>895</v>
       </c>
@@ -9285,7 +9306,7 @@
       </c>
     </row>
     <row r="14" spans="1:11" ht="28.8">
-      <c r="A14" s="203"/>
+      <c r="A14" s="202"/>
       <c r="B14" s="70" t="s">
         <v>896</v>
       </c>
@@ -9313,7 +9334,7 @@
       </c>
     </row>
     <row r="15" spans="1:11" ht="28.8">
-      <c r="A15" s="203"/>
+      <c r="A15" s="202"/>
       <c r="B15" s="70" t="s">
         <v>897</v>
       </c>
@@ -9341,10 +9362,10 @@
       </c>
     </row>
     <row r="16" spans="1:11" ht="43.2">
-      <c r="A16" s="203" t="s">
+      <c r="A16" s="202" t="s">
         <v>898</v>
       </c>
-      <c r="B16" s="203"/>
+      <c r="B16" s="202"/>
       <c r="C16" s="70" t="s">
         <v>930</v>
       </c>
@@ -9758,7 +9779,7 @@
         <v>213</v>
       </c>
       <c r="C3" s="72" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="D3" s="71"/>
       <c r="E3" s="71"/>
@@ -9775,10 +9796,10 @@
         <v>214</v>
       </c>
       <c r="C4" s="72" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="E4" s="71"/>
       <c r="F4" s="71"/>
@@ -9794,7 +9815,7 @@
         <v>215</v>
       </c>
       <c r="C5" s="72" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="D5" s="71"/>
       <c r="E5" s="71"/>
@@ -9811,7 +9832,7 @@
         <v>216</v>
       </c>
       <c r="C6" s="72" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="D6" s="71"/>
       <c r="E6" s="71"/>
@@ -9882,7 +9903,7 @@
         <v>0</v>
       </c>
       <c r="D2" s="67" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="E2" s="68"/>
       <c r="F2" s="68"/>
@@ -9937,13 +9958,13 @@
         <v>295</v>
       </c>
       <c r="B5" s="69" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="C5" s="69" t="s">
         <v>296</v>
       </c>
       <c r="D5" s="64" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="E5" s="69" t="s">
         <v>291</v>
@@ -10073,7 +10094,7 @@
         <v>316</v>
       </c>
       <c r="D11" s="64" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="E11" s="69"/>
       <c r="F11" s="69"/>
@@ -10092,7 +10113,7 @@
         <v>318</v>
       </c>
       <c r="D12" s="64" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="E12" s="69"/>
       <c r="F12" s="69"/>
@@ -10124,13 +10145,13 @@
         <v>323</v>
       </c>
       <c r="B14" s="64" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="C14" s="64" t="s">
         <v>324</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="E14" s="64"/>
       <c r="F14" s="64"/>
@@ -10168,7 +10189,7 @@
         <v>329</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="E16" s="64"/>
       <c r="F16" s="64"/>
@@ -10187,7 +10208,7 @@
         <v>332</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="E17" s="64"/>
       <c r="F17" s="64"/>
@@ -10520,7 +10541,7 @@
         <v>90</v>
       </c>
       <c r="B3" s="69" t="s">
-        <v>1277</v>
+        <v>1275</v>
       </c>
       <c r="C3" s="64" t="s">
         <v>89</v>
@@ -11927,7 +11948,7 @@
         <v>72</v>
       </c>
       <c r="B31" s="13" t="s">
-        <v>1283</v>
+        <v>1281</v>
       </c>
       <c r="C31" s="13" t="s">
         <v>29</v>
@@ -12032,7 +12053,7 @@
         <v>440</v>
       </c>
       <c r="D3" s="64" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="E3" s="69" t="s">
         <v>442</v>
@@ -12081,13 +12102,13 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="69" t="s">
+        <v>1110</v>
+      </c>
+      <c r="B5" s="69" t="s">
         <v>1111</v>
       </c>
-      <c r="B5" s="69" t="s">
-        <v>1112</v>
-      </c>
       <c r="C5" s="64" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
       <c r="D5" s="64"/>
       <c r="E5" s="69" t="s">
@@ -12117,7 +12138,7 @@
         <v>449</v>
       </c>
       <c r="D6" s="64" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="E6" s="69" t="s">
         <v>442</v>
@@ -12195,13 +12216,13 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="69" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="B9" s="69" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="C9" s="64" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
       <c r="D9" s="64"/>
       <c r="E9" s="69" t="s">
@@ -12225,7 +12246,7 @@
         <v>458</v>
       </c>
       <c r="B10" s="69" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="C10" s="64" t="s">
         <v>459</v>
@@ -12251,13 +12272,13 @@
     </row>
     <row r="11" spans="1:9" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="A11" s="64" t="s">
+        <v>1116</v>
+      </c>
+      <c r="B11" s="69" t="s">
+        <v>1115</v>
+      </c>
+      <c r="C11" s="64" t="s">
         <v>1117</v>
-      </c>
-      <c r="B11" s="69" t="s">
-        <v>1116</v>
-      </c>
-      <c r="C11" s="64" t="s">
-        <v>1118</v>
       </c>
       <c r="D11" s="64"/>
       <c r="E11" s="64"/>
@@ -12277,7 +12298,7 @@
         <v>463</v>
       </c>
       <c r="D12" s="64" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="E12" s="64" t="s">
         <v>442</v>
@@ -12391,7 +12412,7 @@
         <v>477</v>
       </c>
       <c r="D16" s="64" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="E16" s="64" t="s">
         <v>442</v>
@@ -12469,13 +12490,13 @@
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="69" t="s">
+        <v>1118</v>
+      </c>
+      <c r="B19" s="69" t="s">
         <v>1119</v>
       </c>
-      <c r="B19" s="69" t="s">
-        <v>1120</v>
-      </c>
       <c r="C19" s="64" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
       <c r="D19" s="64"/>
       <c r="E19" s="64"/>
@@ -12580,7 +12601,7 @@
         <v>493</v>
       </c>
       <c r="D23" s="64" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="E23" s="64" t="s">
         <v>442</v>
@@ -12603,7 +12624,7 @@
         <v>494</v>
       </c>
       <c r="B24" s="69" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="C24" s="69" t="s">
         <v>496</v>
@@ -12694,7 +12715,7 @@
         <v>503</v>
       </c>
       <c r="D27" s="64" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="E27" s="64" t="s">
         <v>442</v>
@@ -12808,7 +12829,7 @@
         <v>512</v>
       </c>
       <c r="D31" s="64" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="E31" s="64" t="s">
         <v>513</v>
@@ -12866,7 +12887,7 @@
         <v>527</v>
       </c>
       <c r="D33" s="64" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="E33" s="64" t="s">
         <v>442</v>
@@ -12889,10 +12910,10 @@
         <v>528</v>
       </c>
       <c r="B34" s="64" t="s">
-        <v>1284</v>
+        <v>1282</v>
       </c>
       <c r="C34" s="64" t="s">
-        <v>1287</v>
+        <v>1285</v>
       </c>
       <c r="D34" s="64" t="s">
         <v>529</v>
@@ -12916,7 +12937,7 @@
     <row r="35" spans="1:9" ht="28.8">
       <c r="A35" s="69"/>
       <c r="B35" s="64" t="s">
-        <v>1285</v>
+        <v>1283</v>
       </c>
       <c r="C35" s="64"/>
       <c r="D35" s="64"/>
@@ -13039,11 +13060,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85DF78F7-F282-409F-A3BB-6F7024B1FD58}">
   <dimension ref="A1:M71"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D30" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="70" workbookViewId="0">
+      <pane xSplit="3" ySplit="2" topLeftCell="D39" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B34" sqref="B34"/>
+      <selection pane="bottomRight" activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
@@ -13204,7 +13225,7 @@
         <v>552</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>1250</v>
+        <v>1248</v>
       </c>
       <c r="D6" s="38" t="s">
         <v>553</v>
@@ -13234,7 +13255,7 @@
         <v>556</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
       <c r="D7" s="38" t="s">
         <v>441</v>
@@ -13346,13 +13367,13 @@
     </row>
     <row r="11" spans="1:10" ht="41.4">
       <c r="A11" s="144" t="s">
+        <v>1127</v>
+      </c>
+      <c r="B11" s="144" t="s">
         <v>1128</v>
       </c>
-      <c r="B11" s="144" t="s">
-        <v>1129</v>
-      </c>
       <c r="C11" s="15" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="D11" s="38" t="s">
         <v>441</v>
@@ -13375,13 +13396,13 @@
     </row>
     <row r="12" spans="1:10" ht="27.6">
       <c r="A12" s="144" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="B12" s="144" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="D12" s="38" t="s">
         <v>441</v>
@@ -13394,13 +13415,13 @@
     </row>
     <row r="13" spans="1:10" ht="27.6">
       <c r="A13" s="144" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
       <c r="B13" s="144" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
       <c r="D13" s="38" t="s">
         <v>441</v>
@@ -13413,13 +13434,13 @@
     </row>
     <row r="14" spans="1:10" ht="41.4">
       <c r="A14" s="144" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="B14" s="144" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="D14" s="38" t="s">
         <v>441</v>
@@ -13432,13 +13453,13 @@
     </row>
     <row r="15" spans="1:10" ht="41.4">
       <c r="A15" s="144" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="B15" s="144" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="D15" s="38" t="s">
         <v>441</v>
@@ -13451,13 +13472,13 @@
     </row>
     <row r="16" spans="1:10" ht="41.4">
       <c r="A16" s="144" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="B16" s="144" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="D16" s="38" t="s">
         <v>441</v>
@@ -13470,13 +13491,13 @@
     </row>
     <row r="17" spans="1:9" ht="27.6">
       <c r="A17" s="144" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
       <c r="B17" s="144" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="D17" s="38" t="s">
         <v>441</v>
@@ -13489,13 +13510,13 @@
     </row>
     <row r="18" spans="1:9" ht="27.6">
       <c r="A18" s="144" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="B18" s="144" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="D18" s="38" t="s">
         <v>441</v>
@@ -13566,13 +13587,13 @@
     </row>
     <row r="21" spans="1:9" ht="41.4">
       <c r="A21" s="14" t="s">
+        <v>1144</v>
+      </c>
+      <c r="B21" s="14" t="s">
         <v>1145</v>
       </c>
-      <c r="B21" s="14" t="s">
+      <c r="C21" s="15" t="s">
         <v>1146</v>
-      </c>
-      <c r="C21" s="15" t="s">
-        <v>1147</v>
       </c>
       <c r="D21" s="38"/>
       <c r="E21" s="16" t="s">
@@ -13792,16 +13813,16 @@
     </row>
     <row r="29" spans="1:9" ht="336.6">
       <c r="A29" s="140" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="B29" s="140" t="s">
         <v>613</v>
       </c>
       <c r="C29" s="23" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
       <c r="D29" s="43" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="E29" s="24" t="s">
         <v>614</v>
@@ -13877,13 +13898,13 @@
     </row>
     <row r="32" spans="1:9" ht="55.2">
       <c r="A32" s="25" t="s">
+        <v>1228</v>
+      </c>
+      <c r="B32" s="170" t="s">
+        <v>1230</v>
+      </c>
+      <c r="C32" s="23" t="s">
         <v>1229</v>
-      </c>
-      <c r="B32" s="170" t="s">
-        <v>1231</v>
-      </c>
-      <c r="C32" s="23" t="s">
-        <v>1230</v>
       </c>
       <c r="D32" s="43" t="s">
         <v>927</v>
@@ -13899,7 +13920,7 @@
         <v>1000</v>
       </c>
       <c r="B33" s="170" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
       <c r="C33" s="23" t="s">
         <v>617</v>
@@ -13919,10 +13940,10 @@
         <v>624</v>
       </c>
       <c r="C34" s="23" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="D34" s="43" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="E34" s="24" t="s">
         <v>625</v>
@@ -13940,7 +13961,7 @@
         <v>823</v>
       </c>
       <c r="J34" s="89" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="35" spans="1:10">
@@ -14001,7 +14022,7 @@
     </row>
     <row r="37" spans="1:10" ht="244.8">
       <c r="A37" s="140" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
       <c r="B37" s="26" t="s">
         <v>630</v>
@@ -14088,7 +14109,7 @@
         <v>639</v>
       </c>
       <c r="C40" s="23" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
       <c r="D40" s="43" t="s">
         <v>927</v>
@@ -14136,7 +14157,7 @@
         <v>442</v>
       </c>
       <c r="J41" s="89" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="20.399999999999999">
@@ -14179,7 +14200,7 @@
         <v>647</v>
       </c>
       <c r="D43" s="43" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="E43" s="44" t="s">
         <v>442</v>
@@ -14264,7 +14285,7 @@
         <v>654</v>
       </c>
       <c r="D46" s="43" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="E46" s="44" t="s">
         <v>442</v>
@@ -14349,7 +14370,7 @@
         <v>663</v>
       </c>
       <c r="D49" s="43" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
       <c r="E49" s="44" t="s">
         <v>442</v>
@@ -14428,13 +14449,13 @@
         <v>668</v>
       </c>
       <c r="B52" s="22" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="C52" s="23" t="s">
         <v>669</v>
       </c>
       <c r="D52" s="43" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
       <c r="E52" s="44" t="s">
         <v>442</v>
@@ -14457,7 +14478,7 @@
         <v>670</v>
       </c>
       <c r="B53" s="22" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="C53" s="23" t="s">
         <v>617</v>
@@ -14479,7 +14500,7 @@
         <v>442</v>
       </c>
       <c r="J53" s="89" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="54" spans="1:10" ht="20.399999999999999">
@@ -14487,7 +14508,7 @@
         <v>671</v>
       </c>
       <c r="B54" s="22" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
       <c r="C54" s="23" t="s">
         <v>621</v>
@@ -14516,7 +14537,7 @@
         <v>672</v>
       </c>
       <c r="B55" s="22" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
       <c r="C55" s="23" t="s">
         <v>673</v>
@@ -14538,7 +14559,7 @@
         <v>442</v>
       </c>
       <c r="J55" s="89" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="56" spans="1:10" ht="20.399999999999999">
@@ -14546,7 +14567,7 @@
         <v>674</v>
       </c>
       <c r="B56" s="22" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="C56" s="23" t="s">
         <v>621</v>
@@ -14601,13 +14622,13 @@
     </row>
     <row r="58" spans="1:10" ht="41.4">
       <c r="A58" s="28" t="s">
+        <v>1147</v>
+      </c>
+      <c r="B58" s="28" t="s">
+        <v>1149</v>
+      </c>
+      <c r="C58" s="29" t="s">
         <v>1148</v>
-      </c>
-      <c r="B58" s="28" t="s">
-        <v>1150</v>
-      </c>
-      <c r="C58" s="29" t="s">
-        <v>1149</v>
       </c>
       <c r="D58" s="45"/>
       <c r="E58" s="30" t="s">
@@ -14715,13 +14736,13 @@
     </row>
     <row r="62" spans="1:10" ht="41.4">
       <c r="A62" s="28" t="s">
+        <v>1150</v>
+      </c>
+      <c r="B62" s="28" t="s">
         <v>1151</v>
       </c>
-      <c r="B62" s="28" t="s">
+      <c r="C62" s="29" t="s">
         <v>1152</v>
-      </c>
-      <c r="C62" s="29" t="s">
-        <v>1153</v>
       </c>
       <c r="D62" s="45" t="s">
         <v>442</v>
@@ -14802,13 +14823,13 @@
     </row>
     <row r="65" spans="1:13" ht="27.6">
       <c r="A65" s="28" t="s">
+        <v>1153</v>
+      </c>
+      <c r="B65" s="28" t="s">
         <v>1154</v>
       </c>
-      <c r="B65" s="28" t="s">
+      <c r="C65" s="29" t="s">
         <v>1155</v>
-      </c>
-      <c r="C65" s="29" t="s">
-        <v>1156</v>
       </c>
       <c r="D65" s="45"/>
       <c r="E65" s="45" t="s">
@@ -14861,10 +14882,10 @@
         <v>712</v>
       </c>
       <c r="B67" s="145" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="C67" s="32" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
       <c r="D67" s="47" t="s">
         <v>714</v>
@@ -14888,10 +14909,10 @@
     <row r="68" spans="1:13" s="178" customFormat="1">
       <c r="A68" s="172"/>
       <c r="B68" s="173" t="s">
-        <v>1278</v>
+        <v>1276</v>
       </c>
       <c r="C68" s="174" t="s">
-        <v>1279</v>
+        <v>1277</v>
       </c>
       <c r="D68" s="175"/>
       <c r="E68" s="176"/>
@@ -14905,10 +14926,10 @@
     </row>
     <row r="69" spans="1:13">
       <c r="A69" s="31" t="s">
+        <v>1157</v>
+      </c>
+      <c r="B69" s="145" t="s">
         <v>1158</v>
-      </c>
-      <c r="B69" s="145" t="s">
-        <v>1159</v>
       </c>
       <c r="C69" s="32" t="s">
         <v>713</v>
@@ -15005,10 +15026,10 @@
   <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A9" sqref="A9:C9"/>
+      <selection pane="bottomRight" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -15060,19 +15081,19 @@
     </row>
     <row r="3" spans="1:10" ht="43.2">
       <c r="A3" s="158" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
       <c r="B3" s="158" t="s">
-        <v>1235</v>
+        <v>1234</v>
       </c>
       <c r="C3" s="158" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
       <c r="D3" s="159" t="s">
         <v>441</v>
       </c>
       <c r="E3" s="156" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
       <c r="H3" s="150"/>
       <c r="I3" s="150"/>
@@ -15080,13 +15101,13 @@
     </row>
     <row r="4" spans="1:10" ht="28.8">
       <c r="A4" s="158" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
       <c r="B4" s="158" t="s">
-        <v>1236</v>
+        <v>1235</v>
       </c>
       <c r="C4" s="158" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
       <c r="D4" s="159" t="s">
         <v>441</v>
@@ -15106,13 +15127,13 @@
     </row>
     <row r="5" spans="1:10" ht="28.8">
       <c r="A5" s="158" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
       <c r="B5" s="158" t="s">
-        <v>1237</v>
+        <v>1236</v>
       </c>
       <c r="C5" s="158" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="D5" s="159" t="s">
         <v>441</v>
@@ -15128,13 +15149,13 @@
     </row>
     <row r="6" spans="1:10" s="10" customFormat="1" ht="43.2">
       <c r="A6" s="158" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
       <c r="B6" s="158" t="s">
-        <v>1238</v>
+        <v>1237</v>
       </c>
       <c r="C6" s="158" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="D6" s="159" t="s">
         <v>441</v>
@@ -15149,13 +15170,13 @@
     </row>
     <row r="7" spans="1:10" ht="28.8">
       <c r="A7" s="158" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
       <c r="B7" s="158" t="s">
-        <v>1239</v>
+        <v>1238</v>
       </c>
       <c r="C7" s="158" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
       <c r="D7" s="159" t="s">
         <v>441</v>
@@ -15169,13 +15190,13 @@
     </row>
     <row r="8" spans="1:10" ht="28.8">
       <c r="A8" s="158" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
       <c r="B8" s="158" t="s">
-        <v>1240</v>
+        <v>1239</v>
       </c>
       <c r="C8" s="158" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
       <c r="D8" s="159" t="s">
         <v>441</v>
@@ -15188,13 +15209,13 @@
     </row>
     <row r="9" spans="1:10" ht="28.8">
       <c r="A9" s="158" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
       <c r="B9" s="158" t="s">
-        <v>1241</v>
+        <v>1240</v>
       </c>
       <c r="C9" s="158" t="s">
-        <v>1182</v>
+        <v>1181</v>
       </c>
       <c r="D9" s="159" t="s">
         <v>441</v>
@@ -15207,13 +15228,13 @@
     </row>
     <row r="10" spans="1:10" ht="28.8">
       <c r="A10" s="158" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
       <c r="B10" s="158" t="s">
-        <v>1242</v>
+        <v>1241</v>
       </c>
       <c r="C10" s="158" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
       <c r="D10" s="159" t="s">
         <v>441</v>
@@ -15226,13 +15247,13 @@
     </row>
     <row r="11" spans="1:10" ht="43.2">
       <c r="A11" s="158" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
       <c r="B11" s="158" t="s">
-        <v>1243</v>
+        <v>1242</v>
       </c>
       <c r="C11" s="158" t="s">
-        <v>1184</v>
+        <v>1183</v>
       </c>
       <c r="D11" s="159" t="s">
         <v>441</v>
@@ -15245,13 +15266,13 @@
     </row>
     <row r="12" spans="1:10" ht="28.8">
       <c r="A12" s="158" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
       <c r="B12" s="158" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="C12" s="158" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
       <c r="D12" s="159" t="s">
         <v>441</v>
@@ -15264,13 +15285,13 @@
     </row>
     <row r="13" spans="1:10" ht="28.8">
       <c r="A13" s="158" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
       <c r="B13" s="158" t="s">
-        <v>1245</v>
+        <v>1288</v>
       </c>
       <c r="C13" s="158" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
       <c r="D13" s="159" t="s">
         <v>441</v>
@@ -15283,10 +15304,10 @@
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="160" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
       <c r="B14" s="160" t="s">
-        <v>1246</v>
+        <v>1244</v>
       </c>
       <c r="C14" s="161" t="s">
         <v>642</v>
@@ -15300,13 +15321,13 @@
     </row>
     <row r="15" spans="1:10" ht="40.799999999999997">
       <c r="A15" s="160" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
       <c r="B15" s="160" t="s">
-        <v>1247</v>
+        <v>1245</v>
       </c>
       <c r="C15" s="161" t="s">
-        <v>1187</v>
+        <v>1186</v>
       </c>
       <c r="D15" s="162" t="s">
         <v>622</v>
@@ -15319,13 +15340,13 @@
     </row>
     <row r="16" spans="1:10" ht="28.8">
       <c r="A16" s="169" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
       <c r="B16" s="169" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
       <c r="C16" s="158" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="D16" s="159" t="s">
         <v>441</v>
@@ -15341,7 +15362,7 @@
         <v>999</v>
       </c>
       <c r="B17" s="161" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
       <c r="C17" s="161"/>
       <c r="D17" s="162"/>
@@ -15353,13 +15374,13 @@
     </row>
     <row r="18" spans="1:9" ht="43.2">
       <c r="A18" s="163" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="B18" s="164" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="C18" s="164" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
       <c r="D18" s="165" t="s">
         <v>441</v>
@@ -15372,13 +15393,13 @@
     </row>
     <row r="19" spans="1:9" ht="43.2">
       <c r="A19" s="163" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="B19" s="164" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
       <c r="C19" s="164" t="s">
-        <v>1202</v>
+        <v>1201</v>
       </c>
       <c r="D19" s="165" t="s">
         <v>441</v>
@@ -15391,13 +15412,13 @@
     </row>
     <row r="20" spans="1:9" ht="43.2">
       <c r="A20" s="163" t="s">
-        <v>1190</v>
+        <v>1189</v>
       </c>
       <c r="B20" s="164" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
       <c r="C20" s="164" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
       <c r="D20" s="165" t="s">
         <v>441</v>
@@ -15410,13 +15431,13 @@
     </row>
     <row r="21" spans="1:9" ht="57.6">
       <c r="A21" s="163" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="B21" s="164" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="C21" s="164" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
       <c r="D21" s="165" t="s">
         <v>441</v>
@@ -15429,13 +15450,13 @@
     </row>
     <row r="22" spans="1:9" ht="43.2">
       <c r="A22" s="163" t="s">
-        <v>1192</v>
+        <v>1191</v>
       </c>
       <c r="B22" s="164" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="C22" s="164" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
       <c r="D22" s="165" t="s">
         <v>441</v>
@@ -15448,13 +15469,13 @@
     </row>
     <row r="23" spans="1:9" ht="43.2">
       <c r="A23" s="163" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
       <c r="B23" s="164" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="C23" s="164" t="s">
-        <v>1206</v>
+        <v>1205</v>
       </c>
       <c r="D23" s="165" t="s">
         <v>441</v>
@@ -15467,13 +15488,13 @@
     </row>
     <row r="24" spans="1:9" ht="43.2">
       <c r="A24" s="163" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
       <c r="B24" s="164" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="C24" s="164" t="s">
-        <v>1207</v>
+        <v>1206</v>
       </c>
       <c r="D24" s="165" t="s">
         <v>441</v>
@@ -15486,13 +15507,13 @@
     </row>
     <row r="25" spans="1:9" ht="57.6">
       <c r="A25" s="163" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
       <c r="B25" s="164" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
       <c r="C25" s="164" t="s">
-        <v>1208</v>
+        <v>1207</v>
       </c>
       <c r="D25" s="165" t="s">
         <v>441</v>
@@ -15505,13 +15526,13 @@
     </row>
     <row r="26" spans="1:9" ht="57.6">
       <c r="A26" s="163" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
       <c r="B26" s="164" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
       <c r="C26" s="164" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
       <c r="D26" s="165" t="s">
         <v>441</v>
@@ -15519,10 +15540,10 @@
     </row>
     <row r="27" spans="1:9">
       <c r="A27" s="166" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="B27" s="167" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
       <c r="C27" s="167" t="s">
         <v>642</v>
@@ -15536,13 +15557,13 @@
     </row>
     <row r="28" spans="1:9" ht="40.799999999999997">
       <c r="A28" s="166" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
       <c r="B28" s="167" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="C28" s="167" t="s">
-        <v>1187</v>
+        <v>1186</v>
       </c>
       <c r="D28" s="168" t="s">
         <v>622</v>
@@ -15567,11 +15588,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8210A5A2-BF82-48DF-82F0-74E3A1B9E934}">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B25" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E25" sqref="E25"/>
+      <selection pane="bottomRight" activeCell="D11" sqref="D11:D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -15603,10 +15624,10 @@
         <v>1001</v>
       </c>
       <c r="C2" s="141" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="D2" s="141" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="E2" s="111" t="s">
         <v>0</v>
@@ -15623,13 +15644,13 @@
         <v>1002</v>
       </c>
       <c r="C3" s="99" t="s">
-        <v>1253</v>
+        <v>1251</v>
       </c>
       <c r="D3" s="192" t="s">
         <v>997</v>
       </c>
       <c r="E3" s="112" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="F3" s="125" t="s">
         <v>996</v>
@@ -15643,11 +15664,11 @@
         <v>442</v>
       </c>
       <c r="C4" s="98" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="D4" s="193"/>
       <c r="E4" s="112" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="F4" s="125"/>
     </row>
@@ -15659,11 +15680,11 @@
         <v>650</v>
       </c>
       <c r="C5" s="99" t="s">
-        <v>1254</v>
+        <v>1252</v>
       </c>
       <c r="D5" s="193"/>
       <c r="E5" s="112" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="F5" s="126"/>
     </row>
@@ -15675,43 +15696,43 @@
         <v>666</v>
       </c>
       <c r="C6" s="99" t="s">
-        <v>1255</v>
+        <v>1253</v>
       </c>
       <c r="D6" s="193"/>
       <c r="E6" s="112" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="F6" s="126"/>
     </row>
     <row r="7" spans="1:6" ht="28.8">
       <c r="A7" s="100" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="B7" s="98" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="C7" s="98" t="s">
-        <v>1256</v>
+        <v>1254</v>
       </c>
       <c r="D7" s="193"/>
       <c r="E7" s="112" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="F7" s="126"/>
     </row>
     <row r="8" spans="1:6" ht="43.2">
       <c r="A8" s="100" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
       <c r="B8" s="98" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="C8" s="98" t="s">
-        <v>1257</v>
+        <v>1255</v>
       </c>
       <c r="D8" s="194"/>
       <c r="E8" s="112" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="F8" s="126"/>
     </row>
@@ -15723,7 +15744,7 @@
         <v>636</v>
       </c>
       <c r="C9" s="97" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="D9" s="191" t="s">
         <v>1003</v>
@@ -15743,7 +15764,7 @@
         <v>658</v>
       </c>
       <c r="C10" s="97" t="s">
-        <v>1259</v>
+        <v>1257</v>
       </c>
       <c r="D10" s="191"/>
       <c r="E10" s="113" t="s">
@@ -15751,7 +15772,7 @@
       </c>
       <c r="F10" s="127"/>
     </row>
-    <row r="11" spans="1:6" ht="28.8">
+    <row r="11" spans="1:6" ht="28.8" customHeight="1">
       <c r="A11" s="101" t="s">
         <v>1007</v>
       </c>
@@ -15759,9 +15780,9 @@
         <v>1011</v>
       </c>
       <c r="C11" s="101" t="s">
-        <v>1260</v>
-      </c>
-      <c r="D11" s="195" t="s">
+        <v>1258</v>
+      </c>
+      <c r="D11" s="204" t="s">
         <v>1042</v>
       </c>
       <c r="E11" s="114" t="s">
@@ -15777,9 +15798,9 @@
         <v>1012</v>
       </c>
       <c r="C12" s="101" t="s">
-        <v>1261</v>
-      </c>
-      <c r="D12" s="195"/>
+        <v>1259</v>
+      </c>
+      <c r="D12" s="205"/>
       <c r="E12" s="114" t="s">
         <v>1032</v>
       </c>
@@ -15793,9 +15814,9 @@
         <v>1013</v>
       </c>
       <c r="C13" s="101" t="s">
-        <v>1262</v>
-      </c>
-      <c r="D13" s="195"/>
+        <v>1260</v>
+      </c>
+      <c r="D13" s="205"/>
       <c r="E13" s="114" t="s">
         <v>1030</v>
       </c>
@@ -15803,105 +15824,107 @@
     </row>
     <row r="14" spans="1:6" ht="28.8">
       <c r="A14" s="101" t="s">
-        <v>1010</v>
+        <v>999</v>
       </c>
       <c r="B14" s="101" t="s">
-        <v>1014</v>
+        <v>442</v>
       </c>
       <c r="C14" s="101" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D14" s="205"/>
+      <c r="E14" s="114" t="s">
+        <v>1033</v>
+      </c>
+      <c r="F14" s="128"/>
+    </row>
+    <row r="15" spans="1:6" ht="43.2">
+      <c r="A15" s="101" t="s">
+        <v>1016</v>
+      </c>
+      <c r="B15" s="101" t="s">
+        <v>1015</v>
+      </c>
+      <c r="C15" s="101" t="s">
+        <v>1262</v>
+      </c>
+      <c r="D15" s="206"/>
+      <c r="E15" s="114" t="s">
+        <v>1034</v>
+      </c>
+      <c r="F15" s="128"/>
+    </row>
+    <row r="16" spans="1:6" s="96" customFormat="1" ht="28.8">
+      <c r="A16" s="108" t="s">
+        <v>1017</v>
+      </c>
+      <c r="B16" s="108" t="s">
+        <v>1019</v>
+      </c>
+      <c r="C16" s="108" t="s">
         <v>1263</v>
       </c>
-      <c r="D14" s="195"/>
-      <c r="E14" s="114" t="s">
-        <v>1031</v>
-      </c>
-      <c r="F14" s="128"/>
-    </row>
-    <row r="15" spans="1:6" ht="28.8">
-      <c r="A15" s="101" t="s">
-        <v>999</v>
-      </c>
-      <c r="B15" s="101" t="s">
-        <v>442</v>
-      </c>
-      <c r="C15" s="101" t="s">
-        <v>1078</v>
-      </c>
-      <c r="D15" s="195"/>
-      <c r="E15" s="114" t="s">
-        <v>1033</v>
-      </c>
-      <c r="F15" s="128"/>
-    </row>
-    <row r="16" spans="1:6" ht="43.2">
-      <c r="A16" s="101" t="s">
-        <v>1016</v>
-      </c>
-      <c r="B16" s="101" t="s">
-        <v>1015</v>
-      </c>
-      <c r="C16" s="101" t="s">
+      <c r="D16" s="195" t="s">
+        <v>1041</v>
+      </c>
+      <c r="E16" s="115" t="s">
+        <v>1067</v>
+      </c>
+      <c r="F16" s="129"/>
+    </row>
+    <row r="17" spans="1:6" s="96" customFormat="1" ht="43.2">
+      <c r="A17" s="108" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B17" s="108" t="s">
+        <v>1021</v>
+      </c>
+      <c r="C17" s="108" t="s">
         <v>1264</v>
       </c>
-      <c r="D16" s="195"/>
-      <c r="E16" s="114" t="s">
-        <v>1034</v>
-      </c>
-      <c r="F16" s="128"/>
-    </row>
-    <row r="17" spans="1:6" s="96" customFormat="1" ht="28.8">
-      <c r="A17" s="108" t="s">
-        <v>1017</v>
-      </c>
-      <c r="B17" s="108" t="s">
-        <v>1019</v>
-      </c>
-      <c r="C17" s="108" t="s">
-        <v>1265</v>
-      </c>
-      <c r="D17" s="196" t="s">
-        <v>1041</v>
-      </c>
+      <c r="D17" s="195"/>
       <c r="E17" s="115" t="s">
         <v>1068</v>
       </c>
       <c r="F17" s="129"/>
     </row>
     <row r="18" spans="1:6" s="96" customFormat="1" ht="43.2">
-      <c r="A18" s="108" t="s">
-        <v>1018</v>
-      </c>
-      <c r="B18" s="108" t="s">
-        <v>1021</v>
-      </c>
-      <c r="C18" s="108" t="s">
-        <v>1266</v>
-      </c>
-      <c r="D18" s="196"/>
-      <c r="E18" s="115" t="s">
+      <c r="A18" s="138" t="s">
+        <v>1022</v>
+      </c>
+      <c r="B18" s="139" t="s">
+        <v>1023</v>
+      </c>
+      <c r="C18" s="139" t="s">
+        <v>1265</v>
+      </c>
+      <c r="D18" s="103" t="s">
+        <v>1040</v>
+      </c>
+      <c r="E18" s="102" t="s">
         <v>1069</v>
       </c>
-      <c r="F18" s="129"/>
-    </row>
-    <row r="19" spans="1:6" s="96" customFormat="1" ht="43.2">
-      <c r="A19" s="138" t="s">
-        <v>1022</v>
-      </c>
-      <c r="B19" s="139" t="s">
-        <v>1023</v>
-      </c>
-      <c r="C19" s="139" t="s">
-        <v>1267</v>
-      </c>
-      <c r="D19" s="103" t="s">
-        <v>1040</v>
-      </c>
-      <c r="E19" s="102" t="s">
-        <v>1070</v>
-      </c>
-      <c r="F19" s="130"/>
-    </row>
-    <row r="20" spans="1:6" s="96" customFormat="1" ht="28.8">
+      <c r="F18" s="130"/>
+    </row>
+    <row r="19" spans="1:6" ht="28.8" customHeight="1">
+      <c r="A19" s="109" t="s">
+        <v>1010</v>
+      </c>
+      <c r="B19" s="109" t="s">
+        <v>1014</v>
+      </c>
+      <c r="C19" s="109" t="s">
+        <v>1261</v>
+      </c>
+      <c r="D19" s="196" t="s">
+        <v>1039</v>
+      </c>
+      <c r="E19" s="116" t="s">
+        <v>1031</v>
+      </c>
+      <c r="F19" s="131"/>
+    </row>
+    <row r="20" spans="1:6" s="96" customFormat="1" ht="28.8" customHeight="1">
       <c r="A20" s="109" t="s">
         <v>1024</v>
       </c>
@@ -15909,11 +15932,9 @@
         <v>1043</v>
       </c>
       <c r="C20" s="109" t="s">
-        <v>1268</v>
-      </c>
-      <c r="D20" s="197" t="s">
-        <v>1039</v>
-      </c>
+        <v>1266</v>
+      </c>
+      <c r="D20" s="197"/>
       <c r="E20" s="116" t="s">
         <v>1035</v>
       </c>
@@ -15927,9 +15948,9 @@
         <v>1044</v>
       </c>
       <c r="C21" s="109" t="s">
-        <v>1269</v>
-      </c>
-      <c r="D21" s="198"/>
+        <v>1267</v>
+      </c>
+      <c r="D21" s="197"/>
       <c r="E21" s="116" t="s">
         <v>1036</v>
       </c>
@@ -15943,9 +15964,9 @@
         <v>1045</v>
       </c>
       <c r="C22" s="109" t="s">
-        <v>1270</v>
-      </c>
-      <c r="D22" s="198"/>
+        <v>1268</v>
+      </c>
+      <c r="D22" s="197"/>
       <c r="E22" s="116" t="s">
         <v>1037</v>
       </c>
@@ -15959,9 +15980,9 @@
         <v>1046</v>
       </c>
       <c r="C23" s="109" t="s">
-        <v>1271</v>
-      </c>
-      <c r="D23" s="199"/>
+        <v>1269</v>
+      </c>
+      <c r="D23" s="198"/>
       <c r="E23" s="116" t="s">
         <v>1038</v>
       </c>
@@ -15975,13 +15996,13 @@
         <v>1020</v>
       </c>
       <c r="C24" s="105" t="s">
-        <v>1272</v>
+        <v>1270</v>
       </c>
       <c r="D24" s="106" t="s">
         <v>1047</v>
       </c>
       <c r="E24" s="117" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="F24" s="132"/>
     </row>
@@ -15993,7 +16014,7 @@
         <v>1050</v>
       </c>
       <c r="C25" s="110" t="s">
-        <v>1273</v>
+        <v>1271</v>
       </c>
       <c r="D25" s="187" t="s">
         <v>1056</v>
@@ -16011,7 +16032,7 @@
         <v>1051</v>
       </c>
       <c r="C26" s="110" t="s">
-        <v>1274</v>
+        <v>1272</v>
       </c>
       <c r="D26" s="187"/>
       <c r="E26" s="118" t="s">
@@ -16027,7 +16048,7 @@
         <v>1053</v>
       </c>
       <c r="C27" s="107" t="s">
-        <v>1275</v>
+        <v>1273</v>
       </c>
       <c r="D27" s="104" t="s">
         <v>1057</v>
@@ -16045,13 +16066,13 @@
         <v>1060</v>
       </c>
       <c r="C28" s="124" t="s">
-        <v>1276</v>
+        <v>1274</v>
       </c>
       <c r="D28" s="188" t="s">
-        <v>1063</v>
+        <v>1286</v>
       </c>
       <c r="E28" s="124" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="F28" s="135"/>
     </row>
@@ -16063,18 +16084,23 @@
         <v>1062</v>
       </c>
       <c r="C29" s="124" t="s">
-        <v>1272</v>
+        <v>1270</v>
       </c>
       <c r="D29" s="189"/>
       <c r="E29" s="124" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="F29" s="135"/>
     </row>
-    <row r="30" spans="1:6" s="96" customFormat="1">
-      <c r="D30" s="122"/>
-      <c r="E30" s="120"/>
-      <c r="F30" s="136"/>
+    <row r="30" spans="1:6" s="96" customFormat="1" ht="57.6">
+      <c r="A30" s="207"/>
+      <c r="B30" s="207"/>
+      <c r="C30" s="207"/>
+      <c r="D30" s="208" t="s">
+        <v>1287</v>
+      </c>
+      <c r="E30" s="209"/>
+      <c r="F30" s="210"/>
     </row>
     <row r="31" spans="1:6" s="96" customFormat="1">
       <c r="D31" s="122"/>
@@ -16093,9 +16119,9 @@
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="D9:D10"/>
     <mergeCell ref="D3:D8"/>
-    <mergeCell ref="D11:D16"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="D20:D23"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="D11:D15"/>
+    <mergeCell ref="D19:D23"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -16288,18 +16314,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -16321,25 +16347,25 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C4E4CF47-E673-4F26-A959-0B7774EBA194}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="4aae9226-4411-406b-98ce-94e2e69fab2c"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D82FA49E-E684-481F-999C-85E775CBBA65}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C4E4CF47-E673-4F26-A959-0B7774EBA194}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="4aae9226-4411-406b-98ce-94e2e69fab2c"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>